<commit_message>
Added my first button with a message box using CSharp. Baby steps.
</commit_message>
<xml_diff>
--- a/DataSheetOne/DataSheetOne/DataSheetOne.xlsx
+++ b/DataSheetOne/DataSheetOne/DataSheetOne.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6675" windowHeight="3533"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21540" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,6 +71,98 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1BD4D61C31492414C321A40F1557A9B627A7C1"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3440"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1058"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>23812</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>176212</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>614363</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>14288</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="_ActiveXWrapper1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd type="none" w="med" len="med"/>
+                </a14:hiddenLine>
+              </a:ext>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects>
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="808080"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -369,14 +461,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId3" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>23813</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>176213</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>614363</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>14288</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId3" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Button Changes using properties window
</commit_message>
<xml_diff>
--- a/DataSheetOne/DataSheetOne/DataSheetOne.xlsx
+++ b/DataSheetOne/DataSheetOne/DataSheetOne.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repositories\ExcelTest\DataSheetOne\DataSheetOne\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\ExcelTest\DataSheetOne\DataSheetOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21540" windowHeight="9390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20620" windowHeight="8910"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,8 +84,8 @@
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3440"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1058"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3316"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1570"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -97,15 +97,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>23812</xdr:colOff>
+          <xdr:colOff>25400</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>176212</xdr:rowOff>
+          <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>614363</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>14288</xdr:rowOff>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>6350</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -132,27 +132,16 @@
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
-                  <a:tailEnd type="none" w="med" len="med"/>
+                  <a:tailEnd/>
                 </a14:hiddenLine>
-              </a:ext>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
               </a:ext>
             </a:extLst>
           </xdr:spPr>
@@ -466,10 +455,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -482,15 +471,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>23813</xdr:colOff>
+                <xdr:colOff>25400</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>176213</xdr:rowOff>
+                <xdr:rowOff>177800</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>614363</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>14288</xdr:rowOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>6350</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>

</xml_diff>